<commit_message>
fix Vertical band horizontal merge regions
</commit_message>
<xml_diff>
--- a/core/modules/core/test/smoketest/test.xlsx
+++ b/core/modules/core/test/smoketest/test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="15120" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="15120" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="data with charts" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
   <definedNames>
     <definedName name="Band1">'data with charts'!$A$1:$C$1</definedName>
     <definedName name="Band2">'data with charts'!$D$1:$F$2</definedName>
-    <definedName name="Band3">'data with charts'!$A$3:$A$4</definedName>
+    <definedName name="Band3">'data with charts'!$A$3:$B$4</definedName>
     <definedName name="Footer">'data with charts'!$A$6:$V$22</definedName>
     <definedName name="Second">charts!$A$1:$K$18</definedName>
     <definedName name="Split">'data with charts'!$A$5:$C$5</definedName>
@@ -126,12 +126,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -235,7 +237,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000311" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000311" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000333" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000333" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -277,24 +279,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="45511424"/>
-        <c:axId val="45512960"/>
+        <c:axId val="78713984"/>
+        <c:axId val="78715520"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="45511424"/>
+        <c:axId val="78713984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="45512960"/>
+        <c:crossAx val="78715520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="45512960"/>
+        <c:axId val="78715520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -302,7 +304,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="45511424"/>
+        <c:crossAx val="78713984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -315,7 +317,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000144" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000144" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -325,9 +327,7 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="ru-RU"/>
   <c:chart>
-    <c:title>
-      <c:layout/>
-    </c:title>
+    <c:title/>
     <c:plotArea>
       <c:layout/>
       <c:pieChart>
@@ -397,7 +397,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:txPr>
         <a:bodyPr/>
         <a:lstStyle/>
@@ -413,7 +412,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000333" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000333" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000355" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000355" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -806,8 +805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:V22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:V22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -825,10 +824,10 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8"/>
+      <c r="E1" s="7"/>
       <c r="F1" s="4" t="s">
         <v>2</v>
       </c>
@@ -841,25 +840,27 @@
       <c r="F2" s="4"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="9" t="s">
         <v>0</v>
       </c>
+      <c r="B3" s="9"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="9" t="s">
         <v>1</v>
       </c>
+      <c r="B4" s="9"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:6" ht="108.75" customHeight="1">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
@@ -878,9 +879,11 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId1"/>
@@ -892,245 +895,245 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="7"/>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
+      <c r="A1" s="6"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
     </row>
     <row r="3" spans="1:11">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
     </row>
     <row r="4" spans="1:11">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
     </row>
     <row r="5" spans="1:11">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
     </row>
     <row r="6" spans="1:11">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
     </row>
     <row r="7" spans="1:11">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
     </row>
     <row r="8" spans="1:11">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
     </row>
     <row r="9" spans="1:11">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
     </row>
     <row r="10" spans="1:11">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
     </row>
     <row r="12" spans="1:11">
-      <c r="A12" s="7"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7"/>
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
     </row>
     <row r="14" spans="1:11">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="7"/>
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
     </row>
     <row r="15" spans="1:11">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="7"/>
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7"/>
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
     </row>
     <row r="17" spans="1:11">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="7"/>
+      <c r="A17" s="6"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
     </row>
     <row r="18" spans="1:11">
-      <c r="A18" s="7"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="7"/>
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fix for long columns (AA, AB, etc)
</commit_message>
<xml_diff>
--- a/core/modules/core/test/smoketest/test.xlsx
+++ b/core/modules/core/test/smoketest/test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="15120" windowHeight="8010"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="15120" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="data with charts" sheetId="1" r:id="rId1"/>
@@ -175,7 +175,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'data with charts'!$B$1</c:f>
+              <c:f>'data with charts'!$C$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -205,7 +205,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'data with charts'!$B$1</c:f>
+              <c:f>'data with charts'!$C$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -237,7 +237,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000333" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000333" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000355" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000355" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -279,24 +279,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="78713984"/>
-        <c:axId val="78715520"/>
+        <c:axId val="65985920"/>
+        <c:axId val="66454656"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="78713984"/>
+        <c:axId val="65985920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="78715520"/>
+        <c:crossAx val="66454656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="78715520"/>
+        <c:axId val="66454656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -304,7 +304,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="78713984"/>
+        <c:crossAx val="65985920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -317,7 +317,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000144" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000144" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000167" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000167" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -327,7 +327,9 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="ru-RU"/>
   <c:chart>
-    <c:title/>
+    <c:title>
+      <c:layout/>
+    </c:title>
     <c:plotArea>
       <c:layout/>
       <c:pieChart>
@@ -351,7 +353,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'data with charts'!$B$1</c:f>
+              <c:f>'data with charts'!$C$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -381,7 +383,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'data with charts'!$B$1</c:f>
+              <c:f>'data with charts'!$C$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -397,6 +399,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:txPr>
         <a:bodyPr/>
         <a:lstStyle/>
@@ -412,7 +415,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000355" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000355" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000377" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000377" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -805,7 +808,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:V22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:B4"/>
     </sheetView>
   </sheetViews>
@@ -895,7 +898,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
PL-6958 Support dynamic styles for XLSX templates
</commit_message>
<xml_diff>
--- a/core/modules/core/test/smoketest/test.xlsx
+++ b/core/modules/core/test/smoketest/test.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="15120" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="15120" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="data with charts" sheetId="1" r:id="rId1"/>
@@ -15,6 +15,7 @@
     <definedName name="Band2">'data with charts'!$D$1:$F$2</definedName>
     <definedName name="Band3">'data with charts'!$A$3:$B$4</definedName>
     <definedName name="Footer">'data with charts'!$A$6:$V$22</definedName>
+    <definedName name="hint_style_theStyle">'data with charts'!$A$1</definedName>
     <definedName name="Second">charts!$A$1:$K$18</definedName>
     <definedName name="Split">'data with charts'!$A$5:$C$5</definedName>
   </definedNames>
@@ -46,8 +47,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -80,8 +81,16 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -100,8 +109,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39994506668294322"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -109,9 +124,25 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -121,12 +152,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -137,21 +168,39 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="theTest" xfId="1"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:pieChart>
@@ -216,12 +265,22 @@
             </c:numRef>
           </c:val>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
         <c:firstSliceAng val="0"/>
       </c:pieChart>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
         <a:lstStyle/>
@@ -234,6 +293,8 @@
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -245,12 +306,24 @@
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -277,34 +350,51 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="65985920"/>
-        <c:axId val="66454656"/>
+        <c:smooth val="0"/>
+        <c:axId val="82361344"/>
+        <c:axId val="82367232"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="65985920"/>
+        <c:axId val="82361344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="66454656"/>
+        <c:crossAx val="82367232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="66454656"/>
+        <c:axId val="82367232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="65985920"/>
+        <c:crossAx val="82361344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -312,8 +402,11 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -325,11 +418,22 @@
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:pieChart>
@@ -394,12 +498,21 @@
             </c:numRef>
           </c:val>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
         <c:firstSliceAng val="0"/>
       </c:pieChart>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
+      <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
         <a:lstStyle/>
@@ -412,6 +525,8 @@
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -596,6 +711,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -630,6 +746,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -805,44 +922,42 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="7"/>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
-      <c r="D2" s="4" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="4"/>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="E2" s="4"/>
+      <c r="F2" s="3"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>0</v>
       </c>
@@ -850,7 +965,7 @@
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>1</v>
       </c>
@@ -858,14 +973,14 @@
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:6" ht="108.75" customHeight="1">
+    <row r="5" spans="1:6" ht="108.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -876,7 +991,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="22:22">
+    <row r="22" spans="22:22" x14ac:dyDescent="0.25">
       <c r="V22" t="s">
         <v>5</v>
       </c>
@@ -895,248 +1010,248 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11">
-      <c r="A1" s="6"/>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-    </row>
-    <row r="2" spans="1:11">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-    </row>
-    <row r="6" spans="1:11">
-      <c r="A6" s="6"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-    </row>
-    <row r="7" spans="1:11">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-    </row>
-    <row r="8" spans="1:11">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-    </row>
-    <row r="9" spans="1:11">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-    </row>
-    <row r="10" spans="1:11">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-    </row>
-    <row r="11" spans="1:11">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-    </row>
-    <row r="12" spans="1:11">
-      <c r="A12" s="6"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-    </row>
-    <row r="13" spans="1:11">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="6"/>
-    </row>
-    <row r="14" spans="1:11">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
-    </row>
-    <row r="15" spans="1:11">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
-      <c r="K15" s="6"/>
-    </row>
-    <row r="16" spans="1:11">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="6"/>
-    </row>
-    <row r="17" spans="1:11">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="6"/>
-      <c r="K17" s="6"/>
-    </row>
-    <row r="18" spans="1:11">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="6"/>
-      <c r="K18" s="6"/>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="5"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>